<commit_message>
Small changes to final output excel file
</commit_message>
<xml_diff>
--- a/FinalOutput.xlsx
+++ b/FinalOutput.xlsx
@@ -412,7 +412,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J188"/>
+  <dimension ref="A1:K188"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -428,45 +428,50 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
+          <t>New Product / Product ID</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
           <t>In price changed?</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>InPriceNew</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>InPriceBefore</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="F1" t="inlineStr">
         <is>
           <t>Out price change?</t>
         </is>
       </c>
-      <c r="F1" t="inlineStr">
+      <c r="G1" t="inlineStr">
         <is>
           <t>OutPriceNew</t>
         </is>
       </c>
-      <c r="G1" t="inlineStr">
+      <c r="H1" t="inlineStr">
         <is>
           <t>OutPriceBefore</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="I1" t="inlineStr">
         <is>
           <t>Season changed?</t>
         </is>
       </c>
-      <c r="I1" t="inlineStr">
+      <c r="J1" t="inlineStr">
         <is>
           <t>SeasonNew</t>
         </is>
       </c>
-      <c r="J1" t="inlineStr">
+      <c r="K1" t="inlineStr">
         <is>
           <t>SeasonBefore</t>
         </is>
@@ -483,13 +488,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C2" t="n">
+      <c r="D2" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F2" t="n">
+      <c r="G2" t="n">
         <v>1399</v>
       </c>
-      <c r="I2" t="inlineStr">
+      <c r="J2" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -506,13 +511,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C3" t="n">
+      <c r="D3" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F3" t="n">
+      <c r="G3" t="n">
         <v>1399</v>
       </c>
-      <c r="I3" t="inlineStr">
+      <c r="J3" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -529,13 +534,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C4" t="n">
+      <c r="D4" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F4" t="n">
+      <c r="G4" t="n">
         <v>1399</v>
       </c>
-      <c r="I4" t="inlineStr">
+      <c r="J4" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -552,13 +557,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C5" t="n">
+      <c r="D5" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F5" t="n">
+      <c r="G5" t="n">
         <v>1399</v>
       </c>
-      <c r="I5" t="inlineStr">
+      <c r="J5" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -575,13 +580,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C6" t="n">
+      <c r="D6" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F6" t="n">
+      <c r="G6" t="n">
         <v>1399</v>
       </c>
-      <c r="I6" t="inlineStr">
+      <c r="J6" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -598,13 +603,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C7" t="n">
+      <c r="D7" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F7" t="n">
+      <c r="G7" t="n">
         <v>1399</v>
       </c>
-      <c r="I7" t="inlineStr">
+      <c r="J7" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -621,13 +626,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C8" t="n">
+      <c r="D8" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F8" t="n">
+      <c r="G8" t="n">
         <v>1399</v>
       </c>
-      <c r="I8" t="inlineStr">
+      <c r="J8" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -644,13 +649,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C9" t="n">
+      <c r="D9" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F9" t="n">
+      <c r="G9" t="n">
         <v>1399</v>
       </c>
-      <c r="I9" t="inlineStr">
+      <c r="J9" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -667,13 +672,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C10" t="n">
+      <c r="D10" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F10" t="n">
+      <c r="G10" t="n">
         <v>1399</v>
       </c>
-      <c r="I10" t="inlineStr">
+      <c r="J10" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -690,13 +695,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C11" t="n">
+      <c r="D11" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F11" t="n">
+      <c r="G11" t="n">
         <v>1399</v>
       </c>
-      <c r="I11" t="inlineStr">
+      <c r="J11" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -713,13 +718,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C12" t="n">
+      <c r="D12" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F12" t="n">
+      <c r="G12" t="n">
         <v>1399</v>
       </c>
-      <c r="I12" t="inlineStr">
+      <c r="J12" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -736,13 +741,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C13" t="n">
+      <c r="D13" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F13" t="n">
+      <c r="G13" t="n">
         <v>1399</v>
       </c>
-      <c r="I13" t="inlineStr">
+      <c r="J13" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -759,13 +764,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C14" t="n">
+      <c r="D14" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F14" t="n">
+      <c r="G14" t="n">
         <v>1399</v>
       </c>
-      <c r="I14" t="inlineStr">
+      <c r="J14" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -782,13 +787,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C15" t="n">
+      <c r="D15" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F15" t="n">
+      <c r="G15" t="n">
         <v>1399</v>
       </c>
-      <c r="I15" t="inlineStr">
+      <c r="J15" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -805,13 +810,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C16" t="n">
+      <c r="D16" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F16" t="n">
+      <c r="G16" t="n">
         <v>1399</v>
       </c>
-      <c r="I16" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -828,13 +833,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C17" t="n">
+      <c r="D17" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F17" t="n">
+      <c r="G17" t="n">
         <v>1399</v>
       </c>
-      <c r="I17" t="inlineStr">
+      <c r="J17" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -851,13 +856,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C18" t="n">
+      <c r="D18" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F18" t="n">
+      <c r="G18" t="n">
         <v>1399</v>
       </c>
-      <c r="I18" t="inlineStr">
+      <c r="J18" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -874,13 +879,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C19" t="n">
+      <c r="D19" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F19" t="n">
+      <c r="G19" t="n">
         <v>1399</v>
       </c>
-      <c r="I19" t="inlineStr">
+      <c r="J19" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -897,13 +902,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C20" t="n">
+      <c r="D20" t="n">
         <v>443.7</v>
       </c>
-      <c r="F20" t="n">
+      <c r="G20" t="n">
         <v>1199</v>
       </c>
-      <c r="I20" t="inlineStr">
+      <c r="J20" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -920,13 +925,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C21" t="n">
+      <c r="D21" t="n">
         <v>443.7</v>
       </c>
-      <c r="F21" t="n">
+      <c r="G21" t="n">
         <v>1199</v>
       </c>
-      <c r="I21" t="inlineStr">
+      <c r="J21" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -943,13 +948,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C22" t="n">
+      <c r="D22" t="n">
         <v>443.7</v>
       </c>
-      <c r="F22" t="n">
+      <c r="G22" t="n">
         <v>1199</v>
       </c>
-      <c r="I22" t="inlineStr">
+      <c r="J22" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -966,13 +971,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C23" t="n">
+      <c r="D23" t="n">
         <v>443.7</v>
       </c>
-      <c r="F23" t="n">
+      <c r="G23" t="n">
         <v>1199</v>
       </c>
-      <c r="I23" t="inlineStr">
+      <c r="J23" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -989,13 +994,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C24" t="n">
+      <c r="D24" t="n">
         <v>443.7</v>
       </c>
-      <c r="F24" t="n">
+      <c r="G24" t="n">
         <v>1199</v>
       </c>
-      <c r="I24" t="inlineStr">
+      <c r="J24" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1012,13 +1017,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C25" t="n">
+      <c r="D25" t="n">
         <v>443.7</v>
       </c>
-      <c r="F25" t="n">
+      <c r="G25" t="n">
         <v>1199</v>
       </c>
-      <c r="I25" t="inlineStr">
+      <c r="J25" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1035,13 +1040,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C26" t="n">
+      <c r="D26" t="n">
         <v>443.7</v>
       </c>
-      <c r="F26" t="n">
+      <c r="G26" t="n">
         <v>1199</v>
       </c>
-      <c r="I26" t="inlineStr">
+      <c r="J26" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1058,13 +1063,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C27" t="n">
+      <c r="D27" t="n">
         <v>443.7</v>
       </c>
-      <c r="F27" t="n">
+      <c r="G27" t="n">
         <v>1199</v>
       </c>
-      <c r="I27" t="inlineStr">
+      <c r="J27" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1081,13 +1086,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C28" t="n">
+      <c r="D28" t="n">
         <v>443.7</v>
       </c>
-      <c r="F28" t="n">
+      <c r="G28" t="n">
         <v>1199</v>
       </c>
-      <c r="I28" t="inlineStr">
+      <c r="J28" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1104,13 +1109,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C29" t="n">
+      <c r="D29" t="n">
         <v>443.7</v>
       </c>
-      <c r="F29" t="n">
+      <c r="G29" t="n">
         <v>1199</v>
       </c>
-      <c r="I29" t="inlineStr">
+      <c r="J29" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1125,28 +1130,39 @@
       <c r="B30" t="n">
         <v>9181059</v>
       </c>
-      <c r="C30" t="n">
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D30" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="E30" t="inlineStr">
+      <c r="E30" t="n">
+        <v>528</v>
+      </c>
+      <c r="F30" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F30" t="n">
+      <c r="G30" t="n">
         <v>1399</v>
       </c>
-      <c r="H30" t="inlineStr">
+      <c r="H30" t="n">
+        <v>1399</v>
+      </c>
+      <c r="I30" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="I30" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="J30" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K30" t="inlineStr">
         <is>
           <t>2302 MAIN</t>
         </is>
@@ -1161,28 +1177,39 @@
       <c r="B31" t="n">
         <v>9181059</v>
       </c>
-      <c r="C31" t="n">
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D31" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="E31" t="inlineStr">
+      <c r="E31" t="n">
+        <v>528</v>
+      </c>
+      <c r="F31" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F31" t="n">
+      <c r="G31" t="n">
         <v>1399</v>
       </c>
-      <c r="H31" t="inlineStr">
+      <c r="H31" t="n">
+        <v>1399</v>
+      </c>
+      <c r="I31" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="I31" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="J31" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K31" t="inlineStr">
         <is>
           <t>2302 MAIN</t>
         </is>
@@ -1197,28 +1224,39 @@
       <c r="B32" t="n">
         <v>9181059</v>
       </c>
-      <c r="C32" t="n">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D32" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="E32" t="inlineStr">
+      <c r="E32" t="n">
+        <v>528</v>
+      </c>
+      <c r="F32" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F32" t="n">
+      <c r="G32" t="n">
         <v>1399</v>
       </c>
-      <c r="H32" t="inlineStr">
+      <c r="H32" t="n">
+        <v>1399</v>
+      </c>
+      <c r="I32" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="I32" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="J32" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K32" t="inlineStr">
         <is>
           <t>2302 MAIN</t>
         </is>
@@ -1233,28 +1271,39 @@
       <c r="B33" t="n">
         <v>9181059</v>
       </c>
-      <c r="C33" t="n">
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D33" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="E33" t="inlineStr">
+      <c r="E33" t="n">
+        <v>528</v>
+      </c>
+      <c r="F33" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F33" t="n">
+      <c r="G33" t="n">
         <v>1399</v>
       </c>
-      <c r="H33" t="inlineStr">
+      <c r="H33" t="n">
+        <v>1399</v>
+      </c>
+      <c r="I33" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="I33" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="J33" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K33" t="inlineStr">
         <is>
           <t>2302 MAIN</t>
         </is>
@@ -1271,13 +1320,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C34" t="n">
+      <c r="D34" t="n">
         <v>517.6900000000001</v>
       </c>
-      <c r="F34" t="n">
+      <c r="G34" t="n">
         <v>1399</v>
       </c>
-      <c r="I34" t="inlineStr">
+      <c r="J34" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1292,28 +1341,39 @@
       <c r="B35" t="n">
         <v>9181059</v>
       </c>
-      <c r="C35" t="n">
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D35" t="n">
         <v>528.25</v>
       </c>
-      <c r="E35" t="inlineStr">
+      <c r="E35" t="n">
+        <v>528</v>
+      </c>
+      <c r="F35" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F35" t="n">
+      <c r="G35" t="n">
         <v>1399</v>
       </c>
-      <c r="H35" t="inlineStr">
+      <c r="H35" t="n">
+        <v>1399</v>
+      </c>
+      <c r="I35" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="I35" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="J35" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K35" t="inlineStr">
         <is>
           <t>2302 MAIN</t>
         </is>
@@ -1328,28 +1388,39 @@
       <c r="B36" t="n">
         <v>9181059</v>
       </c>
-      <c r="C36" t="n">
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D36" t="n">
         <v>528.25</v>
       </c>
-      <c r="E36" t="inlineStr">
+      <c r="E36" t="n">
+        <v>528</v>
+      </c>
+      <c r="F36" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F36" t="n">
+      <c r="G36" t="n">
         <v>1399</v>
       </c>
-      <c r="H36" t="inlineStr">
+      <c r="H36" t="n">
+        <v>1399</v>
+      </c>
+      <c r="I36" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="I36" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="J36" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K36" t="inlineStr">
         <is>
           <t>2302 MAIN</t>
         </is>
@@ -1364,28 +1435,39 @@
       <c r="B37" t="n">
         <v>9181059</v>
       </c>
-      <c r="C37" t="n">
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D37" t="n">
         <v>528.25</v>
       </c>
-      <c r="E37" t="inlineStr">
+      <c r="E37" t="n">
+        <v>528</v>
+      </c>
+      <c r="F37" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F37" t="n">
+      <c r="G37" t="n">
         <v>1399</v>
       </c>
-      <c r="H37" t="inlineStr">
+      <c r="H37" t="n">
+        <v>1399</v>
+      </c>
+      <c r="I37" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="I37" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="J37" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K37" t="inlineStr">
         <is>
           <t>2302 MAIN</t>
         </is>
@@ -1400,28 +1482,39 @@
       <c r="B38" t="n">
         <v>9181059</v>
       </c>
-      <c r="C38" t="n">
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D38" t="n">
         <v>528.25</v>
       </c>
-      <c r="E38" t="inlineStr">
+      <c r="E38" t="n">
+        <v>528</v>
+      </c>
+      <c r="F38" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F38" t="n">
+      <c r="G38" t="n">
         <v>1399</v>
       </c>
-      <c r="H38" t="inlineStr">
+      <c r="H38" t="n">
+        <v>1399</v>
+      </c>
+      <c r="I38" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="I38" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
-      </c>
       <c r="J38" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K38" t="inlineStr">
         <is>
           <t>2302 MAIN</t>
         </is>
@@ -1438,13 +1531,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C39" t="n">
+      <c r="D39" t="n">
         <v>528.25</v>
       </c>
-      <c r="F39" t="n">
+      <c r="G39" t="n">
         <v>1399</v>
       </c>
-      <c r="I39" t="inlineStr">
+      <c r="J39" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1459,23 +1552,39 @@
       <c r="B40" t="n">
         <v>7116037</v>
       </c>
-      <c r="C40" t="n">
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D40" t="n">
         <v>93.09999999999999</v>
       </c>
-      <c r="E40" t="inlineStr">
+      <c r="E40" t="n">
+        <v>93</v>
+      </c>
+      <c r="F40" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F40" t="n">
+      <c r="G40" t="n">
         <v>299</v>
       </c>
-      <c r="H40" t="inlineStr">
+      <c r="H40" t="n">
+        <v>299</v>
+      </c>
+      <c r="I40" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="I40" t="inlineStr">
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K40" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1490,23 +1599,39 @@
       <c r="B41" t="n">
         <v>7116037</v>
       </c>
-      <c r="C41" t="n">
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D41" t="n">
         <v>93.09999999999999</v>
       </c>
-      <c r="E41" t="inlineStr">
+      <c r="E41" t="n">
+        <v>93</v>
+      </c>
+      <c r="F41" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F41" t="n">
+      <c r="G41" t="n">
         <v>299</v>
       </c>
-      <c r="H41" t="inlineStr">
+      <c r="H41" t="n">
+        <v>299</v>
+      </c>
+      <c r="I41" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="I41" t="inlineStr">
+      <c r="J41" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K41" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1521,23 +1646,39 @@
       <c r="B42" t="n">
         <v>7116048</v>
       </c>
-      <c r="C42" t="n">
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D42" t="n">
         <v>93.09999999999999</v>
       </c>
-      <c r="E42" t="inlineStr">
+      <c r="E42" t="n">
+        <v>93</v>
+      </c>
+      <c r="F42" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F42" t="n">
+      <c r="G42" t="n">
         <v>299</v>
       </c>
-      <c r="H42" t="inlineStr">
+      <c r="H42" t="n">
+        <v>299</v>
+      </c>
+      <c r="I42" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="I42" t="inlineStr">
+      <c r="J42" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K42" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1552,23 +1693,39 @@
       <c r="B43" t="n">
         <v>7116048</v>
       </c>
-      <c r="C43" t="n">
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D43" t="n">
         <v>93.09999999999999</v>
       </c>
-      <c r="E43" t="inlineStr">
+      <c r="E43" t="n">
+        <v>93</v>
+      </c>
+      <c r="F43" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F43" t="n">
+      <c r="G43" t="n">
         <v>299</v>
       </c>
-      <c r="H43" t="inlineStr">
+      <c r="H43" t="n">
+        <v>299</v>
+      </c>
+      <c r="I43" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="I43" t="inlineStr">
+      <c r="J43" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K43" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1583,23 +1740,39 @@
       <c r="B44" t="n">
         <v>7116037</v>
       </c>
-      <c r="C44" t="n">
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D44" t="n">
         <v>95</v>
       </c>
-      <c r="E44" t="inlineStr">
+      <c r="E44" t="n">
+        <v>93</v>
+      </c>
+      <c r="F44" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F44" t="n">
+      <c r="G44" t="n">
         <v>299</v>
       </c>
-      <c r="H44" t="inlineStr">
+      <c r="H44" t="n">
+        <v>299</v>
+      </c>
+      <c r="I44" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="I44" t="inlineStr">
+      <c r="J44" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K44" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1614,23 +1787,39 @@
       <c r="B45" t="n">
         <v>7116037</v>
       </c>
-      <c r="C45" t="n">
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D45" t="n">
         <v>95</v>
       </c>
-      <c r="E45" t="inlineStr">
+      <c r="E45" t="n">
+        <v>93</v>
+      </c>
+      <c r="F45" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F45" t="n">
+      <c r="G45" t="n">
         <v>299</v>
       </c>
-      <c r="H45" t="inlineStr">
+      <c r="H45" t="n">
+        <v>299</v>
+      </c>
+      <c r="I45" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="I45" t="inlineStr">
+      <c r="J45" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K45" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1645,23 +1834,39 @@
       <c r="B46" t="n">
         <v>7116048</v>
       </c>
-      <c r="C46" t="n">
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D46" t="n">
         <v>95</v>
       </c>
-      <c r="E46" t="inlineStr">
+      <c r="E46" t="n">
+        <v>93</v>
+      </c>
+      <c r="F46" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F46" t="n">
+      <c r="G46" t="n">
         <v>299</v>
       </c>
-      <c r="H46" t="inlineStr">
+      <c r="H46" t="n">
+        <v>299</v>
+      </c>
+      <c r="I46" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="I46" t="inlineStr">
+      <c r="J46" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K46" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1676,23 +1881,39 @@
       <c r="B47" t="n">
         <v>7116048</v>
       </c>
-      <c r="C47" t="n">
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D47" t="n">
         <v>95</v>
       </c>
-      <c r="E47" t="inlineStr">
+      <c r="E47" t="n">
+        <v>93</v>
+      </c>
+      <c r="F47" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F47" t="n">
+      <c r="G47" t="n">
         <v>299</v>
       </c>
-      <c r="H47" t="inlineStr">
+      <c r="H47" t="n">
+        <v>299</v>
+      </c>
+      <c r="I47" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="I47" t="inlineStr">
+      <c r="J47" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="K47" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -1709,13 +1930,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C48" t="n">
+      <c r="D48" t="n">
         <v>665.42</v>
       </c>
-      <c r="F48" t="n">
+      <c r="G48" t="n">
         <v>1799</v>
       </c>
-      <c r="I48" t="inlineStr">
+      <c r="J48" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -1732,13 +1953,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C49" t="n">
+      <c r="D49" t="n">
         <v>665.42</v>
       </c>
-      <c r="F49" t="n">
+      <c r="G49" t="n">
         <v>1799</v>
       </c>
-      <c r="I49" t="inlineStr">
+      <c r="J49" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -1755,13 +1976,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C50" t="n">
+      <c r="D50" t="n">
         <v>665.42</v>
       </c>
-      <c r="F50" t="n">
+      <c r="G50" t="n">
         <v>1799</v>
       </c>
-      <c r="I50" t="inlineStr">
+      <c r="J50" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -1778,13 +1999,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C51" t="n">
+      <c r="D51" t="n">
         <v>679</v>
       </c>
-      <c r="F51" t="n">
+      <c r="G51" t="n">
         <v>1799</v>
       </c>
-      <c r="I51" t="inlineStr">
+      <c r="J51" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -1801,13 +2022,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C52" t="n">
+      <c r="D52" t="n">
         <v>679</v>
       </c>
-      <c r="F52" t="n">
+      <c r="G52" t="n">
         <v>1799</v>
       </c>
-      <c r="I52" t="inlineStr">
+      <c r="J52" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -1824,13 +2045,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C53" t="n">
+      <c r="D53" t="n">
         <v>679</v>
       </c>
-      <c r="F53" t="n">
+      <c r="G53" t="n">
         <v>1799</v>
       </c>
-      <c r="I53" t="inlineStr">
+      <c r="J53" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -1847,13 +2068,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C54" t="n">
+      <c r="D54" t="n">
         <v>679</v>
       </c>
-      <c r="F54" t="n">
+      <c r="G54" t="n">
         <v>1799</v>
       </c>
-      <c r="I54" t="inlineStr">
+      <c r="J54" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -1870,13 +2091,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C55" t="n">
+      <c r="D55" t="n">
         <v>679</v>
       </c>
-      <c r="F55" t="n">
+      <c r="G55" t="n">
         <v>1799</v>
       </c>
-      <c r="I55" t="inlineStr">
+      <c r="J55" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -1893,13 +2114,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C56" t="n">
+      <c r="D56" t="n">
         <v>679</v>
       </c>
-      <c r="F56" t="n">
+      <c r="G56" t="n">
         <v>1799</v>
       </c>
-      <c r="I56" t="inlineStr">
+      <c r="J56" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -1916,13 +2137,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C57" t="n">
+      <c r="D57" t="n">
         <v>679</v>
       </c>
-      <c r="F57" t="n">
+      <c r="G57" t="n">
         <v>1799</v>
       </c>
-      <c r="I57" t="inlineStr">
+      <c r="J57" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -1939,13 +2160,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C58" t="n">
+      <c r="D58" t="n">
         <v>554.6799999999999</v>
       </c>
-      <c r="F58" t="n">
+      <c r="G58" t="n">
         <v>1499</v>
       </c>
-      <c r="I58" t="inlineStr">
+      <c r="J58" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -1962,13 +2183,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C59" t="n">
+      <c r="D59" t="n">
         <v>554.6799999999999</v>
       </c>
-      <c r="F59" t="n">
+      <c r="G59" t="n">
         <v>1499</v>
       </c>
-      <c r="I59" t="inlineStr">
+      <c r="J59" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -1985,13 +2206,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C60" t="n">
+      <c r="D60" t="n">
         <v>554.6799999999999</v>
       </c>
-      <c r="F60" t="n">
+      <c r="G60" t="n">
         <v>1499</v>
       </c>
-      <c r="I60" t="inlineStr">
+      <c r="J60" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2008,13 +2229,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C61" t="n">
+      <c r="D61" t="n">
         <v>566</v>
       </c>
-      <c r="F61" t="n">
+      <c r="G61" t="n">
         <v>1499</v>
       </c>
-      <c r="I61" t="inlineStr">
+      <c r="J61" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2031,13 +2252,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C62" t="n">
+      <c r="D62" t="n">
         <v>566</v>
       </c>
-      <c r="F62" t="n">
+      <c r="G62" t="n">
         <v>1499</v>
       </c>
-      <c r="I62" t="inlineStr">
+      <c r="J62" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2054,13 +2275,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C63" t="n">
+      <c r="D63" t="n">
         <v>566</v>
       </c>
-      <c r="F63" t="n">
+      <c r="G63" t="n">
         <v>1499</v>
       </c>
-      <c r="I63" t="inlineStr">
+      <c r="J63" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2077,13 +2298,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C64" t="n">
+      <c r="D64" t="n">
         <v>566</v>
       </c>
-      <c r="F64" t="n">
+      <c r="G64" t="n">
         <v>1499</v>
       </c>
-      <c r="I64" t="inlineStr">
+      <c r="J64" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2100,13 +2321,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C65" t="n">
+      <c r="D65" t="n">
         <v>566</v>
       </c>
-      <c r="F65" t="n">
+      <c r="G65" t="n">
         <v>1499</v>
       </c>
-      <c r="I65" t="inlineStr">
+      <c r="J65" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2123,13 +2344,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C66" t="n">
+      <c r="D66" t="n">
         <v>566</v>
       </c>
-      <c r="F66" t="n">
+      <c r="G66" t="n">
         <v>1499</v>
       </c>
-      <c r="I66" t="inlineStr">
+      <c r="J66" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2146,13 +2367,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C67" t="n">
+      <c r="D67" t="n">
         <v>566</v>
       </c>
-      <c r="F67" t="n">
+      <c r="G67" t="n">
         <v>1499</v>
       </c>
-      <c r="I67" t="inlineStr">
+      <c r="J67" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2169,13 +2390,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C68" t="n">
+      <c r="D68" t="n">
         <v>610.05</v>
       </c>
-      <c r="F68" t="n">
+      <c r="G68" t="n">
         <v>1699</v>
       </c>
-      <c r="I68" t="inlineStr">
+      <c r="J68" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2192,13 +2413,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C69" t="n">
+      <c r="D69" t="n">
         <v>610.05</v>
       </c>
-      <c r="F69" t="n">
+      <c r="G69" t="n">
         <v>1699</v>
       </c>
-      <c r="I69" t="inlineStr">
+      <c r="J69" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2215,13 +2436,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C70" t="n">
+      <c r="D70" t="n">
         <v>610.05</v>
       </c>
-      <c r="F70" t="n">
+      <c r="G70" t="n">
         <v>1699</v>
       </c>
-      <c r="I70" t="inlineStr">
+      <c r="J70" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2238,13 +2459,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C71" t="n">
+      <c r="D71" t="n">
         <v>610.05</v>
       </c>
-      <c r="F71" t="n">
+      <c r="G71" t="n">
         <v>1699</v>
       </c>
-      <c r="I71" t="inlineStr">
+      <c r="J71" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2261,13 +2482,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C72" t="n">
+      <c r="D72" t="n">
         <v>622.5</v>
       </c>
-      <c r="F72" t="n">
+      <c r="G72" t="n">
         <v>1699</v>
       </c>
-      <c r="I72" t="inlineStr">
+      <c r="J72" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2284,13 +2505,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C73" t="n">
+      <c r="D73" t="n">
         <v>622.5</v>
       </c>
-      <c r="F73" t="n">
+      <c r="G73" t="n">
         <v>1699</v>
       </c>
-      <c r="I73" t="inlineStr">
+      <c r="J73" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2307,13 +2528,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C74" t="n">
+      <c r="D74" t="n">
         <v>622.5</v>
       </c>
-      <c r="F74" t="n">
+      <c r="G74" t="n">
         <v>1699</v>
       </c>
-      <c r="I74" t="inlineStr">
+      <c r="J74" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2330,13 +2551,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C75" t="n">
+      <c r="D75" t="n">
         <v>622.5</v>
       </c>
-      <c r="F75" t="n">
+      <c r="G75" t="n">
         <v>1699</v>
       </c>
-      <c r="I75" t="inlineStr">
+      <c r="J75" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2353,13 +2574,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C76" t="n">
+      <c r="D76" t="n">
         <v>622.5</v>
       </c>
-      <c r="F76" t="n">
+      <c r="G76" t="n">
         <v>1699</v>
       </c>
-      <c r="I76" t="inlineStr">
+      <c r="J76" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2376,13 +2597,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C77" t="n">
+      <c r="D77" t="n">
         <v>622.5</v>
       </c>
-      <c r="F77" t="n">
+      <c r="G77" t="n">
         <v>1699</v>
       </c>
-      <c r="I77" t="inlineStr">
+      <c r="J77" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2399,13 +2620,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C78" t="n">
+      <c r="D78" t="n">
         <v>622.5</v>
       </c>
-      <c r="F78" t="n">
+      <c r="G78" t="n">
         <v>1699</v>
       </c>
-      <c r="I78" t="inlineStr">
+      <c r="J78" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2422,13 +2643,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C79" t="n">
+      <c r="D79" t="n">
         <v>622.5</v>
       </c>
-      <c r="F79" t="n">
+      <c r="G79" t="n">
         <v>1699</v>
       </c>
-      <c r="I79" t="inlineStr">
+      <c r="J79" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2445,13 +2666,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C80" t="n">
+      <c r="D80" t="n">
         <v>622.5</v>
       </c>
-      <c r="F80" t="n">
+      <c r="G80" t="n">
         <v>1699</v>
       </c>
-      <c r="I80" t="inlineStr">
+      <c r="J80" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2468,13 +2689,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C81" t="n">
+      <c r="D81" t="n">
         <v>554.6799999999999</v>
       </c>
-      <c r="F81" t="n">
+      <c r="G81" t="n">
         <v>1499</v>
       </c>
-      <c r="I81" t="inlineStr">
+      <c r="J81" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2491,13 +2712,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C82" t="n">
+      <c r="D82" t="n">
         <v>554.6799999999999</v>
       </c>
-      <c r="F82" t="n">
+      <c r="G82" t="n">
         <v>1499</v>
       </c>
-      <c r="I82" t="inlineStr">
+      <c r="J82" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2514,13 +2735,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C83" t="n">
+      <c r="D83" t="n">
         <v>554.6799999999999</v>
       </c>
-      <c r="F83" t="n">
+      <c r="G83" t="n">
         <v>1499</v>
       </c>
-      <c r="I83" t="inlineStr">
+      <c r="J83" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2537,13 +2758,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C84" t="n">
+      <c r="D84" t="n">
         <v>554.6799999999999</v>
       </c>
-      <c r="F84" t="n">
+      <c r="G84" t="n">
         <v>1499</v>
       </c>
-      <c r="I84" t="inlineStr">
+      <c r="J84" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2560,13 +2781,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C85" t="n">
+      <c r="D85" t="n">
         <v>566</v>
       </c>
-      <c r="F85" t="n">
+      <c r="G85" t="n">
         <v>1499</v>
       </c>
-      <c r="I85" t="inlineStr">
+      <c r="J85" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2583,13 +2804,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C86" t="n">
+      <c r="D86" t="n">
         <v>566</v>
       </c>
-      <c r="F86" t="n">
+      <c r="G86" t="n">
         <v>1499</v>
       </c>
-      <c r="I86" t="inlineStr">
+      <c r="J86" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2606,13 +2827,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C87" t="n">
+      <c r="D87" t="n">
         <v>566</v>
       </c>
-      <c r="F87" t="n">
+      <c r="G87" t="n">
         <v>1499</v>
       </c>
-      <c r="I87" t="inlineStr">
+      <c r="J87" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2629,13 +2850,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C88" t="n">
+      <c r="D88" t="n">
         <v>566</v>
       </c>
-      <c r="F88" t="n">
+      <c r="G88" t="n">
         <v>1499</v>
       </c>
-      <c r="I88" t="inlineStr">
+      <c r="J88" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2652,13 +2873,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C89" t="n">
+      <c r="D89" t="n">
         <v>277.34</v>
       </c>
-      <c r="F89" t="n">
+      <c r="G89" t="n">
         <v>749</v>
       </c>
-      <c r="I89" t="inlineStr">
+      <c r="J89" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2675,13 +2896,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C90" t="n">
+      <c r="D90" t="n">
         <v>277.34</v>
       </c>
-      <c r="F90" t="n">
+      <c r="G90" t="n">
         <v>749</v>
       </c>
-      <c r="I90" t="inlineStr">
+      <c r="J90" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2698,13 +2919,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C91" t="n">
+      <c r="D91" t="n">
         <v>277.34</v>
       </c>
-      <c r="F91" t="n">
+      <c r="G91" t="n">
         <v>749</v>
       </c>
-      <c r="I91" t="inlineStr">
+      <c r="J91" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2721,13 +2942,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C92" t="n">
+      <c r="D92" t="n">
         <v>277.34</v>
       </c>
-      <c r="F92" t="n">
+      <c r="G92" t="n">
         <v>749</v>
       </c>
-      <c r="I92" t="inlineStr">
+      <c r="J92" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2744,13 +2965,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C93" t="n">
+      <c r="D93" t="n">
         <v>277.34</v>
       </c>
-      <c r="F93" t="n">
+      <c r="G93" t="n">
         <v>749</v>
       </c>
-      <c r="I93" t="inlineStr">
+      <c r="J93" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2767,13 +2988,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C94" t="n">
+      <c r="D94" t="n">
         <v>277.34</v>
       </c>
-      <c r="F94" t="n">
+      <c r="G94" t="n">
         <v>749</v>
       </c>
-      <c r="I94" t="inlineStr">
+      <c r="J94" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2790,13 +3011,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C95" t="n">
+      <c r="D95" t="n">
         <v>277.34</v>
       </c>
-      <c r="F95" t="n">
+      <c r="G95" t="n">
         <v>749</v>
       </c>
-      <c r="I95" t="inlineStr">
+      <c r="J95" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2813,13 +3034,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C96" t="n">
+      <c r="D96" t="n">
         <v>277.34</v>
       </c>
-      <c r="F96" t="n">
+      <c r="G96" t="n">
         <v>749</v>
       </c>
-      <c r="I96" t="inlineStr">
+      <c r="J96" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2836,13 +3057,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C97" t="n">
+      <c r="D97" t="n">
         <v>283</v>
       </c>
-      <c r="F97" t="n">
+      <c r="G97" t="n">
         <v>749</v>
       </c>
-      <c r="I97" t="inlineStr">
+      <c r="J97" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2859,13 +3080,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C98" t="n">
+      <c r="D98" t="n">
         <v>283</v>
       </c>
-      <c r="F98" t="n">
+      <c r="G98" t="n">
         <v>749</v>
       </c>
-      <c r="I98" t="inlineStr">
+      <c r="J98" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2882,13 +3103,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C99" t="n">
+      <c r="D99" t="n">
         <v>283</v>
       </c>
-      <c r="F99" t="n">
+      <c r="G99" t="n">
         <v>749</v>
       </c>
-      <c r="I99" t="inlineStr">
+      <c r="J99" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2905,13 +3126,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C100" t="n">
+      <c r="D100" t="n">
         <v>283</v>
       </c>
-      <c r="F100" t="n">
+      <c r="G100" t="n">
         <v>749</v>
       </c>
-      <c r="I100" t="inlineStr">
+      <c r="J100" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2928,13 +3149,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C101" t="n">
+      <c r="D101" t="n">
         <v>283</v>
       </c>
-      <c r="F101" t="n">
+      <c r="G101" t="n">
         <v>749</v>
       </c>
-      <c r="I101" t="inlineStr">
+      <c r="J101" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2951,13 +3172,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C102" t="n">
+      <c r="D102" t="n">
         <v>283</v>
       </c>
-      <c r="F102" t="n">
+      <c r="G102" t="n">
         <v>749</v>
       </c>
-      <c r="I102" t="inlineStr">
+      <c r="J102" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2974,13 +3195,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C103" t="n">
+      <c r="D103" t="n">
         <v>283</v>
       </c>
-      <c r="F103" t="n">
+      <c r="G103" t="n">
         <v>749</v>
       </c>
-      <c r="I103" t="inlineStr">
+      <c r="J103" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -2997,13 +3218,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C104" t="n">
+      <c r="D104" t="n">
         <v>283</v>
       </c>
-      <c r="F104" t="n">
+      <c r="G104" t="n">
         <v>749</v>
       </c>
-      <c r="I104" t="inlineStr">
+      <c r="J104" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3020,13 +3241,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C105" t="n">
+      <c r="D105" t="n">
         <v>264</v>
       </c>
-      <c r="F105" t="n">
+      <c r="G105" t="n">
         <v>699</v>
       </c>
-      <c r="I105" t="inlineStr">
+      <c r="J105" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3043,13 +3264,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C106" t="n">
+      <c r="D106" t="n">
         <v>264</v>
       </c>
-      <c r="F106" t="n">
+      <c r="G106" t="n">
         <v>699</v>
       </c>
-      <c r="I106" t="inlineStr">
+      <c r="J106" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3066,13 +3287,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C107" t="n">
+      <c r="D107" t="n">
         <v>264</v>
       </c>
-      <c r="F107" t="n">
+      <c r="G107" t="n">
         <v>699</v>
       </c>
-      <c r="I107" t="inlineStr">
+      <c r="J107" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3089,13 +3310,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C108" t="n">
+      <c r="D108" t="n">
         <v>264</v>
       </c>
-      <c r="F108" t="n">
+      <c r="G108" t="n">
         <v>699</v>
       </c>
-      <c r="I108" t="inlineStr">
+      <c r="J108" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3112,13 +3333,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C109" t="n">
+      <c r="D109" t="n">
         <v>264</v>
       </c>
-      <c r="F109" t="n">
+      <c r="G109" t="n">
         <v>699</v>
       </c>
-      <c r="I109" t="inlineStr">
+      <c r="J109" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3135,13 +3356,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C110" t="n">
+      <c r="D110" t="n">
         <v>264</v>
       </c>
-      <c r="F110" t="n">
+      <c r="G110" t="n">
         <v>699</v>
       </c>
-      <c r="I110" t="inlineStr">
+      <c r="J110" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3158,13 +3379,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C111" t="n">
+      <c r="D111" t="n">
         <v>264</v>
       </c>
-      <c r="F111" t="n">
+      <c r="G111" t="n">
         <v>699</v>
       </c>
-      <c r="I111" t="inlineStr">
+      <c r="J111" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3181,13 +3402,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C112" t="n">
+      <c r="D112" t="n">
         <v>264</v>
       </c>
-      <c r="F112" t="n">
+      <c r="G112" t="n">
         <v>699</v>
       </c>
-      <c r="I112" t="inlineStr">
+      <c r="J112" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3204,13 +3425,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C113" t="n">
+      <c r="D113" t="n">
         <v>264</v>
       </c>
-      <c r="F113" t="n">
+      <c r="G113" t="n">
         <v>699</v>
       </c>
-      <c r="I113" t="inlineStr">
+      <c r="J113" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3227,13 +3448,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C114" t="n">
+      <c r="D114" t="n">
         <v>264</v>
       </c>
-      <c r="F114" t="n">
+      <c r="G114" t="n">
         <v>699</v>
       </c>
-      <c r="I114" t="inlineStr">
+      <c r="J114" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3248,28 +3469,39 @@
       <c r="B115" t="n">
         <v>7018070</v>
       </c>
-      <c r="C115" t="n">
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D115" t="n">
         <v>339.5</v>
       </c>
-      <c r="E115" t="inlineStr">
+      <c r="E115" t="n">
+        <v>302</v>
+      </c>
+      <c r="F115" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F115" t="n">
+      <c r="G115" t="n">
         <v>899</v>
       </c>
-      <c r="H115" t="inlineStr">
+      <c r="H115" t="n">
+        <v>899</v>
+      </c>
+      <c r="I115" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="I115" t="inlineStr">
-        <is>
-          <t>2401 PRE</t>
-        </is>
-      </c>
       <c r="J115" t="inlineStr">
+        <is>
+          <t>2401 PRE</t>
+        </is>
+      </c>
+      <c r="K115" t="inlineStr">
         <is>
           <t>1</t>
         </is>
@@ -3284,28 +3516,39 @@
       <c r="B116" t="n">
         <v>7018080</v>
       </c>
-      <c r="C116" t="n">
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D116" t="n">
         <v>339.5</v>
       </c>
-      <c r="E116" t="inlineStr">
+      <c r="E116" t="n">
+        <v>185</v>
+      </c>
+      <c r="F116" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F116" t="n">
+      <c r="G116" t="n">
         <v>899</v>
       </c>
-      <c r="H116" t="inlineStr">
+      <c r="H116" t="n">
+        <v>899</v>
+      </c>
+      <c r="I116" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="I116" t="inlineStr">
-        <is>
-          <t>2401 PRE</t>
-        </is>
-      </c>
       <c r="J116" t="inlineStr">
+        <is>
+          <t>2401 PRE</t>
+        </is>
+      </c>
+      <c r="K116" t="inlineStr">
         <is>
           <t>2201 MAIN</t>
         </is>
@@ -3322,13 +3565,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C117" t="n">
+      <c r="D117" t="n">
         <v>339.5</v>
       </c>
-      <c r="F117" t="n">
+      <c r="G117" t="n">
         <v>899</v>
       </c>
-      <c r="I117" t="inlineStr">
+      <c r="J117" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3343,28 +3586,39 @@
       <c r="B118" t="n">
         <v>6525703</v>
       </c>
-      <c r="C118" t="n">
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>Yes</t>
+        </is>
+      </c>
+      <c r="D118" t="n">
         <v>339.5</v>
       </c>
-      <c r="E118" t="inlineStr">
+      <c r="E118" t="n">
+        <v>302</v>
+      </c>
+      <c r="F118" t="inlineStr">
         <is>
           <t>No</t>
         </is>
       </c>
-      <c r="F118" t="n">
+      <c r="G118" t="n">
         <v>899</v>
       </c>
-      <c r="H118" t="inlineStr">
+      <c r="H118" t="n">
+        <v>899</v>
+      </c>
+      <c r="I118" t="inlineStr">
         <is>
           <t>Yes</t>
         </is>
       </c>
-      <c r="I118" t="inlineStr">
-        <is>
-          <t>2401 PRE</t>
-        </is>
-      </c>
       <c r="J118" t="inlineStr">
+        <is>
+          <t>2401 PRE</t>
+        </is>
+      </c>
+      <c r="K118" t="inlineStr">
         <is>
           <t>CARRYOVERS</t>
         </is>
@@ -3381,13 +3635,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C119" t="n">
+      <c r="D119" t="n">
         <v>1396</v>
       </c>
-      <c r="F119" t="n">
+      <c r="G119" t="n">
         <v>3699</v>
       </c>
-      <c r="I119" t="inlineStr">
+      <c r="J119" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3404,13 +3658,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C120" t="n">
+      <c r="D120" t="n">
         <v>1396</v>
       </c>
-      <c r="F120" t="n">
+      <c r="G120" t="n">
         <v>3699</v>
       </c>
-      <c r="I120" t="inlineStr">
+      <c r="J120" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3427,13 +3681,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C121" t="n">
+      <c r="D121" t="n">
         <v>776.41</v>
       </c>
-      <c r="F121" t="n">
+      <c r="G121" t="n">
         <v>2099</v>
       </c>
-      <c r="I121" t="inlineStr">
+      <c r="J121" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3450,13 +3704,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C122" t="n">
+      <c r="D122" t="n">
         <v>776.41</v>
       </c>
-      <c r="F122" t="n">
+      <c r="G122" t="n">
         <v>2099</v>
       </c>
-      <c r="I122" t="inlineStr">
+      <c r="J122" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3473,13 +3727,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C123" t="n">
+      <c r="D123" t="n">
         <v>776.41</v>
       </c>
-      <c r="F123" t="n">
+      <c r="G123" t="n">
         <v>2099</v>
       </c>
-      <c r="I123" t="inlineStr">
+      <c r="J123" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3496,13 +3750,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C124" t="n">
+      <c r="D124" t="n">
         <v>776.41</v>
       </c>
-      <c r="F124" t="n">
+      <c r="G124" t="n">
         <v>2099</v>
       </c>
-      <c r="I124" t="inlineStr">
+      <c r="J124" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3519,13 +3773,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C125" t="n">
+      <c r="D125" t="n">
         <v>776.41</v>
       </c>
-      <c r="F125" t="n">
+      <c r="G125" t="n">
         <v>2099</v>
       </c>
-      <c r="I125" t="inlineStr">
+      <c r="J125" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3542,13 +3796,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C126" t="n">
+      <c r="D126" t="n">
         <v>776.41</v>
       </c>
-      <c r="F126" t="n">
+      <c r="G126" t="n">
         <v>2099</v>
       </c>
-      <c r="I126" t="inlineStr">
+      <c r="J126" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3565,13 +3819,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C127" t="n">
+      <c r="D127" t="n">
         <v>792.25</v>
       </c>
-      <c r="F127" t="n">
+      <c r="G127" t="n">
         <v>2099</v>
       </c>
-      <c r="I127" t="inlineStr">
+      <c r="J127" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3588,13 +3842,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C128" t="n">
+      <c r="D128" t="n">
         <v>792.25</v>
       </c>
-      <c r="F128" t="n">
+      <c r="G128" t="n">
         <v>2099</v>
       </c>
-      <c r="I128" t="inlineStr">
+      <c r="J128" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3611,13 +3865,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C129" t="n">
+      <c r="D129" t="n">
         <v>792.25</v>
       </c>
-      <c r="F129" t="n">
+      <c r="G129" t="n">
         <v>2099</v>
       </c>
-      <c r="I129" t="inlineStr">
+      <c r="J129" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3634,13 +3888,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C130" t="n">
+      <c r="D130" t="n">
         <v>792.25</v>
       </c>
-      <c r="F130" t="n">
+      <c r="G130" t="n">
         <v>2099</v>
       </c>
-      <c r="I130" t="inlineStr">
+      <c r="J130" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3657,13 +3911,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C131" t="n">
+      <c r="D131" t="n">
         <v>792.25</v>
       </c>
-      <c r="F131" t="n">
+      <c r="G131" t="n">
         <v>2099</v>
       </c>
-      <c r="I131" t="inlineStr">
+      <c r="J131" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3680,13 +3934,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C132" t="n">
+      <c r="D132" t="n">
         <v>792.25</v>
       </c>
-      <c r="F132" t="n">
+      <c r="G132" t="n">
         <v>2099</v>
       </c>
-      <c r="I132" t="inlineStr">
+      <c r="J132" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3703,13 +3957,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C133" t="n">
+      <c r="D133" t="n">
         <v>1109.36</v>
       </c>
-      <c r="F133" t="n">
+      <c r="G133" t="n">
         <v>2999</v>
       </c>
-      <c r="I133" t="inlineStr">
+      <c r="J133" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3726,13 +3980,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C134" t="n">
+      <c r="D134" t="n">
         <v>1109.36</v>
       </c>
-      <c r="F134" t="n">
+      <c r="G134" t="n">
         <v>2999</v>
       </c>
-      <c r="I134" t="inlineStr">
+      <c r="J134" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3749,13 +4003,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C135" t="n">
+      <c r="D135" t="n">
         <v>1109.36</v>
       </c>
-      <c r="F135" t="n">
+      <c r="G135" t="n">
         <v>2999</v>
       </c>
-      <c r="I135" t="inlineStr">
+      <c r="J135" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3772,13 +4026,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C136" t="n">
+      <c r="D136" t="n">
         <v>1132</v>
       </c>
-      <c r="F136" t="n">
+      <c r="G136" t="n">
         <v>2999</v>
       </c>
-      <c r="I136" t="inlineStr">
+      <c r="J136" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3795,13 +4049,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C137" t="n">
+      <c r="D137" t="n">
         <v>1132</v>
       </c>
-      <c r="F137" t="n">
+      <c r="G137" t="n">
         <v>2999</v>
       </c>
-      <c r="I137" t="inlineStr">
+      <c r="J137" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3818,13 +4072,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C138" t="n">
+      <c r="D138" t="n">
         <v>1132</v>
       </c>
-      <c r="F138" t="n">
+      <c r="G138" t="n">
         <v>2999</v>
       </c>
-      <c r="I138" t="inlineStr">
+      <c r="J138" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3841,13 +4095,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C139" t="n">
+      <c r="D139" t="n">
         <v>1132</v>
       </c>
-      <c r="F139" t="n">
+      <c r="G139" t="n">
         <v>2999</v>
       </c>
-      <c r="I139" t="inlineStr">
+      <c r="J139" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3864,13 +4118,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C140" t="n">
+      <c r="D140" t="n">
         <v>554.6799999999999</v>
       </c>
-      <c r="F140" t="n">
+      <c r="G140" t="n">
         <v>1499</v>
       </c>
-      <c r="I140" t="inlineStr">
+      <c r="J140" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3887,13 +4141,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C141" t="n">
+      <c r="D141" t="n">
         <v>554.6799999999999</v>
       </c>
-      <c r="F141" t="n">
+      <c r="G141" t="n">
         <v>1499</v>
       </c>
-      <c r="I141" t="inlineStr">
+      <c r="J141" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3910,13 +4164,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C142" t="n">
+      <c r="D142" t="n">
         <v>554.6799999999999</v>
       </c>
-      <c r="F142" t="n">
+      <c r="G142" t="n">
         <v>1499</v>
       </c>
-      <c r="I142" t="inlineStr">
+      <c r="J142" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3933,13 +4187,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C143" t="n">
+      <c r="D143" t="n">
         <v>566</v>
       </c>
-      <c r="F143" t="n">
+      <c r="G143" t="n">
         <v>1499</v>
       </c>
-      <c r="I143" t="inlineStr">
+      <c r="J143" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3956,13 +4210,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C144" t="n">
+      <c r="D144" t="n">
         <v>566</v>
       </c>
-      <c r="F144" t="n">
+      <c r="G144" t="n">
         <v>1499</v>
       </c>
-      <c r="I144" t="inlineStr">
+      <c r="J144" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -3979,13 +4233,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C145" t="n">
+      <c r="D145" t="n">
         <v>566</v>
       </c>
-      <c r="F145" t="n">
+      <c r="G145" t="n">
         <v>1499</v>
       </c>
-      <c r="I145" t="inlineStr">
+      <c r="J145" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4002,13 +4256,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C146" t="n">
+      <c r="D146" t="n">
         <v>1053.75</v>
       </c>
-      <c r="F146" t="n">
+      <c r="G146" t="n">
         <v>2899</v>
       </c>
-      <c r="I146" t="inlineStr">
+      <c r="J146" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4025,13 +4279,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C147" t="n">
+      <c r="D147" t="n">
         <v>1053.75</v>
       </c>
-      <c r="F147" t="n">
+      <c r="G147" t="n">
         <v>2899</v>
       </c>
-      <c r="I147" t="inlineStr">
+      <c r="J147" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4048,13 +4302,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C148" t="n">
+      <c r="D148" t="n">
         <v>1053.75</v>
       </c>
-      <c r="F148" t="n">
+      <c r="G148" t="n">
         <v>2899</v>
       </c>
-      <c r="I148" t="inlineStr">
+      <c r="J148" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4071,13 +4325,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C149" t="n">
+      <c r="D149" t="n">
         <v>1075.25</v>
       </c>
-      <c r="F149" t="n">
+      <c r="G149" t="n">
         <v>2899</v>
       </c>
-      <c r="I149" t="inlineStr">
+      <c r="J149" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4094,13 +4348,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C150" t="n">
+      <c r="D150" t="n">
         <v>1075.25</v>
       </c>
-      <c r="F150" t="n">
+      <c r="G150" t="n">
         <v>2899</v>
       </c>
-      <c r="I150" t="inlineStr">
+      <c r="J150" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4117,13 +4371,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C151" t="n">
+      <c r="D151" t="n">
         <v>1075.25</v>
       </c>
-      <c r="F151" t="n">
+      <c r="G151" t="n">
         <v>2899</v>
       </c>
-      <c r="I151" t="inlineStr">
+      <c r="J151" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4140,13 +4394,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C152" t="n">
+      <c r="D152" t="n">
         <v>1245.25</v>
       </c>
-      <c r="F152" t="n">
+      <c r="G152" t="n">
         <v>3299</v>
       </c>
-      <c r="I152" t="inlineStr">
+      <c r="J152" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4163,13 +4417,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C153" t="n">
+      <c r="D153" t="n">
         <v>1245.25</v>
       </c>
-      <c r="F153" t="n">
+      <c r="G153" t="n">
         <v>3299</v>
       </c>
-      <c r="I153" t="inlineStr">
+      <c r="J153" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4186,13 +4440,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C154" t="n">
+      <c r="D154" t="n">
         <v>1245.25</v>
       </c>
-      <c r="F154" t="n">
+      <c r="G154" t="n">
         <v>3299</v>
       </c>
-      <c r="I154" t="inlineStr">
+      <c r="J154" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4209,13 +4463,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C155" t="n">
+      <c r="D155" t="n">
         <v>332.71</v>
       </c>
-      <c r="F155" t="n">
+      <c r="G155" t="n">
         <v>899</v>
       </c>
-      <c r="I155" t="inlineStr">
+      <c r="J155" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4232,13 +4486,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C156" t="n">
+      <c r="D156" t="n">
         <v>332.71</v>
       </c>
-      <c r="F156" t="n">
+      <c r="G156" t="n">
         <v>899</v>
       </c>
-      <c r="I156" t="inlineStr">
+      <c r="J156" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4255,13 +4509,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C157" t="n">
+      <c r="D157" t="n">
         <v>332.71</v>
       </c>
-      <c r="F157" t="n">
+      <c r="G157" t="n">
         <v>899</v>
       </c>
-      <c r="I157" t="inlineStr">
+      <c r="J157" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4278,13 +4532,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C158" t="n">
+      <c r="D158" t="n">
         <v>332.71</v>
       </c>
-      <c r="F158" t="n">
+      <c r="G158" t="n">
         <v>899</v>
       </c>
-      <c r="I158" t="inlineStr">
+      <c r="J158" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4301,13 +4555,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C159" t="n">
+      <c r="D159" t="n">
         <v>339.5</v>
       </c>
-      <c r="F159" t="n">
+      <c r="G159" t="n">
         <v>899</v>
       </c>
-      <c r="I159" t="inlineStr">
+      <c r="J159" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4324,13 +4578,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C160" t="n">
+      <c r="D160" t="n">
         <v>339.5</v>
       </c>
-      <c r="F160" t="n">
+      <c r="G160" t="n">
         <v>899</v>
       </c>
-      <c r="I160" t="inlineStr">
+      <c r="J160" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4347,13 +4601,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C161" t="n">
+      <c r="D161" t="n">
         <v>339.5</v>
       </c>
-      <c r="F161" t="n">
+      <c r="G161" t="n">
         <v>899</v>
       </c>
-      <c r="I161" t="inlineStr">
+      <c r="J161" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4370,13 +4624,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C162" t="n">
+      <c r="D162" t="n">
         <v>339.5</v>
       </c>
-      <c r="F162" t="n">
+      <c r="G162" t="n">
         <v>899</v>
       </c>
-      <c r="I162" t="inlineStr">
+      <c r="J162" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4393,13 +4647,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C163" t="n">
+      <c r="D163" t="n">
         <v>339.5</v>
       </c>
-      <c r="F163" t="n">
+      <c r="G163" t="n">
         <v>899</v>
       </c>
-      <c r="I163" t="inlineStr">
+      <c r="J163" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4416,13 +4670,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C164" t="n">
+      <c r="D164" t="n">
         <v>339.5</v>
       </c>
-      <c r="F164" t="n">
+      <c r="G164" t="n">
         <v>899</v>
       </c>
-      <c r="I164" t="inlineStr">
+      <c r="J164" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4439,13 +4693,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C165" t="n">
+      <c r="D165" t="n">
         <v>339.5</v>
       </c>
-      <c r="F165" t="n">
+      <c r="G165" t="n">
         <v>899</v>
       </c>
-      <c r="I165" t="inlineStr">
+      <c r="J165" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4462,13 +4716,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C166" t="n">
+      <c r="D166" t="n">
         <v>339.5</v>
       </c>
-      <c r="F166" t="n">
+      <c r="G166" t="n">
         <v>899</v>
       </c>
-      <c r="I166" t="inlineStr">
+      <c r="J166" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4485,13 +4739,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C167" t="n">
+      <c r="D167" t="n">
         <v>443.7</v>
       </c>
-      <c r="F167" t="n">
+      <c r="G167" t="n">
         <v>1199</v>
       </c>
-      <c r="I167" t="inlineStr">
+      <c r="J167" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4508,13 +4762,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C168" t="n">
+      <c r="D168" t="n">
         <v>443.7</v>
       </c>
-      <c r="F168" t="n">
+      <c r="G168" t="n">
         <v>1199</v>
       </c>
-      <c r="I168" t="inlineStr">
+      <c r="J168" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4531,13 +4785,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C169" t="n">
+      <c r="D169" t="n">
         <v>443.7</v>
       </c>
-      <c r="F169" t="n">
+      <c r="G169" t="n">
         <v>1199</v>
       </c>
-      <c r="I169" t="inlineStr">
+      <c r="J169" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4554,13 +4808,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C170" t="n">
+      <c r="D170" t="n">
         <v>452.75</v>
       </c>
-      <c r="F170" t="n">
+      <c r="G170" t="n">
         <v>1199</v>
       </c>
-      <c r="I170" t="inlineStr">
+      <c r="J170" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4577,13 +4831,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C171" t="n">
+      <c r="D171" t="n">
         <v>452.75</v>
       </c>
-      <c r="F171" t="n">
+      <c r="G171" t="n">
         <v>1199</v>
       </c>
-      <c r="I171" t="inlineStr">
+      <c r="J171" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4600,13 +4854,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C172" t="n">
+      <c r="D172" t="n">
         <v>452.75</v>
       </c>
-      <c r="F172" t="n">
+      <c r="G172" t="n">
         <v>1199</v>
       </c>
-      <c r="I172" t="inlineStr">
+      <c r="J172" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4623,13 +4877,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C173" t="n">
+      <c r="D173" t="n">
         <v>452.75</v>
       </c>
-      <c r="F173" t="n">
+      <c r="G173" t="n">
         <v>1199</v>
       </c>
-      <c r="I173" t="inlineStr">
+      <c r="J173" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4646,13 +4900,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C174" t="n">
+      <c r="D174" t="n">
         <v>776.41</v>
       </c>
-      <c r="F174" t="n">
+      <c r="G174" t="n">
         <v>2099</v>
       </c>
-      <c r="I174" t="inlineStr">
+      <c r="J174" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4669,13 +4923,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C175" t="n">
+      <c r="D175" t="n">
         <v>776.41</v>
       </c>
-      <c r="F175" t="n">
+      <c r="G175" t="n">
         <v>2099</v>
       </c>
-      <c r="I175" t="inlineStr">
+      <c r="J175" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4692,13 +4946,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C176" t="n">
+      <c r="D176" t="n">
         <v>776.41</v>
       </c>
-      <c r="F176" t="n">
+      <c r="G176" t="n">
         <v>2099</v>
       </c>
-      <c r="I176" t="inlineStr">
+      <c r="J176" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4715,13 +4969,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C177" t="n">
+      <c r="D177" t="n">
         <v>776.41</v>
       </c>
-      <c r="F177" t="n">
+      <c r="G177" t="n">
         <v>2099</v>
       </c>
-      <c r="I177" t="inlineStr">
+      <c r="J177" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4738,13 +4992,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C178" t="n">
+      <c r="D178" t="n">
         <v>776.41</v>
       </c>
-      <c r="F178" t="n">
+      <c r="G178" t="n">
         <v>2099</v>
       </c>
-      <c r="I178" t="inlineStr">
+      <c r="J178" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4761,13 +5015,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C179" t="n">
+      <c r="D179" t="n">
         <v>776.41</v>
       </c>
-      <c r="F179" t="n">
+      <c r="G179" t="n">
         <v>2099</v>
       </c>
-      <c r="I179" t="inlineStr">
+      <c r="J179" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4784,13 +5038,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C180" t="n">
+      <c r="D180" t="n">
         <v>776.41</v>
       </c>
-      <c r="F180" t="n">
+      <c r="G180" t="n">
         <v>2099</v>
       </c>
-      <c r="I180" t="inlineStr">
+      <c r="J180" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4807,13 +5061,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C181" t="n">
+      <c r="D181" t="n">
         <v>792.25</v>
       </c>
-      <c r="F181" t="n">
+      <c r="G181" t="n">
         <v>2099</v>
       </c>
-      <c r="I181" t="inlineStr">
+      <c r="J181" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4830,13 +5084,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C182" t="n">
+      <c r="D182" t="n">
         <v>792.25</v>
       </c>
-      <c r="F182" t="n">
+      <c r="G182" t="n">
         <v>2099</v>
       </c>
-      <c r="I182" t="inlineStr">
+      <c r="J182" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4853,13 +5107,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C183" t="n">
+      <c r="D183" t="n">
         <v>792.25</v>
       </c>
-      <c r="F183" t="n">
+      <c r="G183" t="n">
         <v>2099</v>
       </c>
-      <c r="I183" t="inlineStr">
+      <c r="J183" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4876,13 +5130,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C184" t="n">
+      <c r="D184" t="n">
         <v>792.25</v>
       </c>
-      <c r="F184" t="n">
+      <c r="G184" t="n">
         <v>2099</v>
       </c>
-      <c r="I184" t="inlineStr">
+      <c r="J184" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4899,13 +5153,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C185" t="n">
+      <c r="D185" t="n">
         <v>792.25</v>
       </c>
-      <c r="F185" t="n">
+      <c r="G185" t="n">
         <v>2099</v>
       </c>
-      <c r="I185" t="inlineStr">
+      <c r="J185" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4922,13 +5176,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C186" t="n">
+      <c r="D186" t="n">
         <v>792.25</v>
       </c>
-      <c r="F186" t="n">
+      <c r="G186" t="n">
         <v>2099</v>
       </c>
-      <c r="I186" t="inlineStr">
+      <c r="J186" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4945,13 +5199,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C187" t="n">
+      <c r="D187" t="n">
         <v>792.25</v>
       </c>
-      <c r="F187" t="n">
+      <c r="G187" t="n">
         <v>2099</v>
       </c>
-      <c r="I187" t="inlineStr">
+      <c r="J187" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>
@@ -4968,13 +5222,13 @@
           <t>New product</t>
         </is>
       </c>
-      <c r="C188" t="n">
+      <c r="D188" t="n">
         <v>792.25</v>
       </c>
-      <c r="F188" t="n">
+      <c r="G188" t="n">
         <v>2099</v>
       </c>
-      <c r="I188" t="inlineStr">
+      <c r="J188" t="inlineStr">
         <is>
           <t>2401 PRE</t>
         </is>

</xml_diff>